<commit_message>
Cập nhật danh sach
</commit_message>
<xml_diff>
--- a/DanhsachCN.xlsx
+++ b/DanhsachCN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Workspaces\BieuMau\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA4AE0B-BBC1-48F5-9D8C-1EE0C76DF4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B673D87C-CED3-4970-BB08-B5357CD9401B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="403">
   <si>
     <t>Thủ Đức</t>
   </si>
@@ -1274,13 +1274,31 @@
   </si>
   <si>
     <t>Tên chi nhánh cũ</t>
+  </si>
+  <si>
+    <t>Cty 1: Hà Nội; 
+Công ty 5: Bắc cạn, Bắc Giang, Bắc Ninh, Cao Bằng, Hưng Yên, Hải Dương, Hải Phòng, Lạng Sơn, Quảng Ninh, Thái Bình, Thái Nguyên</t>
+  </si>
+  <si>
+    <t>Cty 3: Bình Định, Huế, Quảng Nam,, Quảng Ngãi, Quảng Trị, Đà Nẵng
+Cty 4: Hà Giang, Hà Nam, Hòa Bình, Lai Châu, Lào Cai, Nam Định, Ninh Bình, Phú Thọ, Sơn La, Tuyên Quang, Vĩnh Phúc, Yên Bái, Điện Biên</t>
+  </si>
+  <si>
+    <t>Cty 6: Hà Tĩnh, Nghệ An, Quảng Bình, Thanh Hóa
+Cty 7: Phú Yên, Gia Lai, Khánh Hòa, KonTum, Đack Lak, Đack Nông</t>
+  </si>
+  <si>
+    <t>Cty 9: An Giang, Bạc Liêu, Bến Tre, Cà Mau, Cần Thơ, Hậu Giang, Kiên Giang, Phú Quốc, Sóc Trăng, Tiền Giang, Trà Vinh, Vĩnh Long, Đồng Tháp</t>
+  </si>
+  <si>
+    <t>Cty 8: Bình Dương, Bình Phước, Bình Thuận, Long An, Lâm Đồng, Ninh Thuận, Tây Ninh, Vũng Tàu, Đồng Nai</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1323,8 +1341,14 @@
       <color rgb="FFFF0000"/>
       <name val="&quot;Times New Roman&quot;"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1343,8 +1367,14 @@
         <bgColor rgb="FFF1F1F1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1391,11 +1421,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1425,6 +1483,34 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1643,11 +1729,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G169"/>
+  <dimension ref="A1:G174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F113" sqref="F113"/>
+      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F174" sqref="F174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -5124,88 +5210,158 @@
       <c r="G165" s="1"/>
     </row>
     <row r="166" spans="1:7">
-      <c r="A166" s="4">
+      <c r="A166" s="11">
         <v>165</v>
       </c>
-      <c r="B166" s="5" t="s">
+      <c r="B166" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="C166" s="5" t="s">
+      <c r="C166" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="D166" s="6" t="s">
+      <c r="D166" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="E166" s="6" t="s">
+      <c r="E166" s="13" t="s">
         <v>365</v>
       </c>
-      <c r="F166" s="6" t="s">
+      <c r="F166" s="13" t="s">
         <v>390</v>
       </c>
       <c r="G166" s="1"/>
     </row>
     <row r="167" spans="1:7">
-      <c r="A167" s="4">
+      <c r="A167" s="14">
         <v>166</v>
       </c>
-      <c r="B167" s="5" t="s">
+      <c r="B167" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="C167" s="5" t="s">
+      <c r="C167" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="D167" s="6" t="s">
+      <c r="D167" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="E167" s="6" t="s">
+      <c r="E167" s="16" t="s">
         <v>372</v>
       </c>
-      <c r="F167" s="6" t="s">
+      <c r="F167" s="16" t="s">
         <v>392</v>
       </c>
       <c r="G167" s="1"/>
     </row>
     <row r="168" spans="1:7">
-      <c r="A168" s="4">
+      <c r="A168" s="14">
         <v>167</v>
       </c>
-      <c r="B168" s="5" t="s">
+      <c r="B168" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="C168" s="5" t="s">
+      <c r="C168" s="15" t="s">
         <v>393</v>
       </c>
-      <c r="D168" s="6" t="s">
+      <c r="D168" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="E168" s="6" t="s">
+      <c r="E168" s="16" t="s">
         <v>365</v>
       </c>
-      <c r="F168" s="6" t="s">
+      <c r="F168" s="16" t="s">
         <v>394</v>
       </c>
       <c r="G168" s="1"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="4">
+      <c r="A169" s="14">
         <v>168</v>
       </c>
-      <c r="B169" s="5" t="s">
+      <c r="B169" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="C169" s="5" t="s">
+      <c r="C169" s="15" t="s">
         <v>395</v>
       </c>
-      <c r="D169" s="6" t="s">
+      <c r="D169" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="E169" s="6" t="s">
+      <c r="E169" s="16" t="s">
         <v>361</v>
       </c>
-      <c r="F169" s="6" t="s">
+      <c r="F169" s="16" t="s">
         <v>396</v>
       </c>
       <c r="G169" s="1"/>
+    </row>
+    <row r="170" spans="1:7" ht="15" customHeight="1">
+      <c r="A170" s="17">
+        <v>169</v>
+      </c>
+      <c r="B170" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C170" s="19"/>
+      <c r="D170" s="19"/>
+      <c r="E170" s="19"/>
+      <c r="F170" s="20" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" ht="15" customHeight="1">
+      <c r="A171" s="14">
+        <v>170</v>
+      </c>
+      <c r="B171" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C171" s="19"/>
+      <c r="D171" s="19"/>
+      <c r="E171" s="19"/>
+      <c r="F171" s="20" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" ht="15" customHeight="1">
+      <c r="A172" s="14">
+        <v>171</v>
+      </c>
+      <c r="B172" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C172" s="19"/>
+      <c r="D172" s="19"/>
+      <c r="E172" s="19"/>
+      <c r="F172" s="20" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="15" customHeight="1">
+      <c r="A173" s="17">
+        <v>172</v>
+      </c>
+      <c r="B173" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="C173" s="19"/>
+      <c r="D173" s="19"/>
+      <c r="E173" s="19"/>
+      <c r="F173" s="20" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" ht="15" customHeight="1">
+      <c r="A174" s="14">
+        <v>173</v>
+      </c>
+      <c r="B174" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C174" s="19"/>
+      <c r="D174" s="19"/>
+      <c r="E174" s="19"/>
+      <c r="F174" s="20" t="s">
+        <v>402</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>